<commit_message>
r script and predictions updated
</commit_message>
<xml_diff>
--- a/cherry_predictions_JF.xlsx
+++ b/cherry_predictions_JF.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="12">
   <si>
     <t>MAE for lm(bloom_doy ~ year)</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">MAE for rf(bloom_doy ~ .) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAE for gbm(bloom_doy ~ .) </t>
   </si>
 </sst>
 </file>
@@ -890,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,19 +906,24 @@
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -923,22 +931,29 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -954,38 +969,53 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1001,38 +1031,53 @@
       <c r="E3" s="1">
         <v>3.13</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2011</v>
       </c>
       <c r="I3" s="1">
+        <v>99</v>
+      </c>
+      <c r="J3" s="1">
+        <v>95.08</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3.92</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="1">
         <v>2011</v>
       </c>
-      <c r="J3" s="1">
+      <c r="O3" s="1">
         <v>99</v>
       </c>
-      <c r="K3" s="1">
-        <v>95.08</v>
-      </c>
-      <c r="L3" s="1">
-        <v>3.92</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P3" s="1">
+        <v>97.31</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1.69</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="1">
         <v>2011</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="U3" s="1">
         <v>99</v>
       </c>
-      <c r="R3" s="1">
-        <v>97.31</v>
-      </c>
-      <c r="S3" s="1">
-        <v>1.69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V3" s="1">
+        <v>96.42</v>
+      </c>
+      <c r="W3" s="1">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1048,38 +1093,53 @@
       <c r="E4" s="1">
         <v>7.07</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>8</v>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2011</v>
       </c>
       <c r="I4" s="1">
+        <v>90</v>
+      </c>
+      <c r="J4" s="1">
+        <v>91.02</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="1">
         <v>2011</v>
       </c>
-      <c r="J4" s="1">
+      <c r="O4" s="1">
         <v>90</v>
       </c>
-      <c r="K4" s="1">
-        <v>91.02</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1.02</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P4" s="1">
+        <v>88.38</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="1">
         <v>2011</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="U4" s="1">
         <v>90</v>
       </c>
-      <c r="R4" s="1">
-        <v>88.38</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V4" s="1">
+        <v>87.72</v>
+      </c>
+      <c r="W4" s="1">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1095,38 +1155,53 @@
       <c r="E5" s="1">
         <v>3.55</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>9</v>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2011</v>
       </c>
       <c r="I5" s="1">
+        <v>88</v>
+      </c>
+      <c r="J5" s="1">
+        <v>91.08</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3.08</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="1">
         <v>2011</v>
       </c>
-      <c r="J5" s="1">
+      <c r="O5" s="1">
         <v>88</v>
       </c>
-      <c r="K5" s="1">
-        <v>91.08</v>
-      </c>
-      <c r="L5" s="1">
-        <v>3.08</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P5" s="1">
+        <v>92.28</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>4.28</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="1">
         <v>2011</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="U5" s="1">
         <v>88</v>
       </c>
-      <c r="R5" s="1">
-        <v>92.28</v>
-      </c>
-      <c r="S5" s="1">
-        <v>4.28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V5" s="1">
+        <v>88.7</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0.70000000000000295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1142,38 +1217,53 @@
       <c r="E6" s="1">
         <v>5.12</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>7</v>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2012</v>
       </c>
       <c r="I6" s="1">
+        <v>101</v>
+      </c>
+      <c r="J6" s="1">
+        <v>93.98</v>
+      </c>
+      <c r="K6" s="1">
+        <v>7.02</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="1">
         <v>2012</v>
       </c>
-      <c r="J6" s="1">
+      <c r="O6" s="1">
         <v>101</v>
       </c>
-      <c r="K6" s="1">
-        <v>93.98</v>
-      </c>
-      <c r="L6" s="1">
-        <v>7.02</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P6" s="1">
+        <v>99</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>2</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" s="1">
         <v>2012</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="U6" s="1">
         <v>101</v>
       </c>
-      <c r="R6" s="1">
-        <v>99</v>
-      </c>
-      <c r="S6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V6" s="1">
+        <v>99.22</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1189,38 +1279,53 @@
       <c r="E7" s="1">
         <v>3.74</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>8</v>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2012</v>
       </c>
       <c r="I7" s="1">
+        <v>93</v>
+      </c>
+      <c r="J7" s="1">
+        <v>94.91</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.91</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="1">
         <v>2012</v>
       </c>
-      <c r="J7" s="1">
+      <c r="O7" s="1">
         <v>93</v>
       </c>
-      <c r="K7" s="1">
-        <v>94.91</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1.91</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P7" s="1">
+        <v>91.2</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="1">
         <v>2012</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="U7" s="1">
         <v>93</v>
       </c>
-      <c r="R7" s="1">
-        <v>91.2</v>
-      </c>
-      <c r="S7" s="1">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V7" s="1">
+        <v>91.94</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1236,38 +1341,53 @@
       <c r="E8" s="1">
         <v>11.34</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2012</v>
       </c>
       <c r="I8" s="1">
+        <v>80</v>
+      </c>
+      <c r="J8" s="1">
+        <v>96.36</v>
+      </c>
+      <c r="K8" s="1">
+        <v>16.36</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="1">
         <v>2012</v>
       </c>
-      <c r="J8" s="1">
+      <c r="O8" s="1">
         <v>80</v>
       </c>
-      <c r="K8" s="1">
-        <v>96.36</v>
-      </c>
-      <c r="L8" s="1">
-        <v>16.36</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P8" s="1">
+        <v>88.82</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>8.8199999999999896</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T8" s="1">
         <v>2012</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="U8" s="1">
         <v>80</v>
       </c>
-      <c r="R8" s="1">
-        <v>88.82</v>
-      </c>
-      <c r="S8" s="1">
-        <v>8.8199999999999896</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V8" s="1">
+        <v>85.62</v>
+      </c>
+      <c r="W8" s="1">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1283,38 +1403,53 @@
       <c r="E9" s="1">
         <v>2.95</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>7</v>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2013</v>
       </c>
       <c r="I9" s="1">
+        <v>93</v>
+      </c>
+      <c r="J9" s="1">
+        <v>93.37</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="1">
         <v>2013</v>
       </c>
-      <c r="J9" s="1">
+      <c r="O9" s="1">
         <v>93</v>
       </c>
-      <c r="K9" s="1">
-        <v>93.37</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0.37</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P9" s="1">
+        <v>94.6</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1.5999999999999901</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T9" s="1">
         <v>2013</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="U9" s="1">
         <v>93</v>
       </c>
-      <c r="R9" s="1">
-        <v>94.6</v>
-      </c>
-      <c r="S9" s="1">
-        <v>1.5999999999999901</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V9" s="1">
+        <v>93.16</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.15999999999999701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1330,38 +1465,53 @@
       <c r="E10" s="1">
         <v>10.47</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>8</v>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2013</v>
       </c>
       <c r="I10" s="1">
+        <v>107</v>
+      </c>
+      <c r="J10" s="1">
+        <v>104.36</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2.64</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="1">
         <v>2013</v>
       </c>
-      <c r="J10" s="1">
+      <c r="O10" s="1">
         <v>107</v>
       </c>
-      <c r="K10" s="1">
-        <v>104.36</v>
-      </c>
-      <c r="L10" s="1">
-        <v>2.64</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P10" s="1">
+        <v>104.77</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2.23</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
         <v>2013</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="U10" s="1">
         <v>107</v>
       </c>
-      <c r="R10" s="1">
-        <v>104.77</v>
-      </c>
-      <c r="S10" s="1">
-        <v>2.23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V10" s="1">
+        <v>106.06</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.93999999999999795</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1377,38 +1527,53 @@
       <c r="E11" s="1">
         <v>8.2100000000000009</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>9</v>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2013</v>
       </c>
       <c r="I11" s="1">
+        <v>99</v>
+      </c>
+      <c r="J11" s="1">
+        <v>94.35</v>
+      </c>
+      <c r="K11" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="1">
         <v>2013</v>
       </c>
-      <c r="J11" s="1">
+      <c r="O11" s="1">
         <v>99</v>
       </c>
-      <c r="K11" s="1">
-        <v>94.35</v>
-      </c>
-      <c r="L11" s="1">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P11" s="1">
+        <v>97.95</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" s="1">
         <v>2013</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="U11" s="1">
         <v>99</v>
       </c>
-      <c r="R11" s="1">
-        <v>97.95</v>
-      </c>
-      <c r="S11" s="1">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V11" s="1">
+        <v>98.03</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0.96999999999999897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1424,38 +1589,53 @@
       <c r="E12" s="1">
         <v>1.78</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>7</v>
+      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2014</v>
       </c>
       <c r="I12" s="1">
+        <v>94</v>
+      </c>
+      <c r="J12" s="1">
+        <v>94.38</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="1">
         <v>2014</v>
       </c>
-      <c r="J12" s="1">
+      <c r="O12" s="1">
         <v>94</v>
       </c>
-      <c r="K12" s="1">
-        <v>94.38</v>
-      </c>
-      <c r="L12" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P12" s="1">
+        <v>95.2</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T12" s="1">
         <v>2014</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="U12" s="1">
         <v>94</v>
       </c>
-      <c r="R12" s="1">
-        <v>95.2</v>
-      </c>
-      <c r="S12" s="1">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V12" s="1">
+        <v>94.16</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.15999999999999701</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1471,38 +1651,53 @@
       <c r="E13" s="1">
         <v>12.79</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>8</v>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2014</v>
       </c>
       <c r="I13" s="1">
+        <v>84</v>
+      </c>
+      <c r="J13" s="1">
+        <v>94.96</v>
+      </c>
+      <c r="K13" s="1">
+        <v>10.96</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" s="1">
         <v>2014</v>
       </c>
-      <c r="J13" s="1">
+      <c r="O13" s="1">
         <v>84</v>
       </c>
-      <c r="K13" s="1">
-        <v>94.96</v>
-      </c>
-      <c r="L13" s="1">
-        <v>10.96</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P13" s="1">
+        <v>87.43</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>3.4300000000000099</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T13" s="1">
         <v>2014</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="U13" s="1">
         <v>84</v>
       </c>
-      <c r="R13" s="1">
-        <v>87.43</v>
-      </c>
-      <c r="S13" s="1">
-        <v>3.4300000000000099</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V13" s="1">
+        <v>86.16</v>
+      </c>
+      <c r="W13" s="1">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1518,38 +1713,53 @@
       <c r="E14" s="1">
         <v>8.93</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>9</v>
+      <c r="G14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2014</v>
       </c>
       <c r="I14" s="1">
+        <v>100</v>
+      </c>
+      <c r="J14" s="1">
+        <v>94.02</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5.98</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="1">
         <v>2014</v>
       </c>
-      <c r="J14" s="1">
+      <c r="O14" s="1">
         <v>100</v>
       </c>
-      <c r="K14" s="1">
-        <v>94.02</v>
-      </c>
-      <c r="L14" s="1">
-        <v>5.98</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P14" s="1">
+        <v>101.39</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1.39</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T14" s="1">
         <v>2014</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="U14" s="1">
         <v>100</v>
       </c>
-      <c r="R14" s="1">
-        <v>101.39</v>
-      </c>
-      <c r="S14" s="1">
-        <v>1.39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V14" s="1">
+        <v>105.57</v>
+      </c>
+      <c r="W14" s="1">
+        <v>5.5699999999999896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1565,38 +1775,53 @@
       <c r="E15" s="1">
         <v>2.65</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>7</v>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2015</v>
       </c>
       <c r="I15" s="1">
+        <v>93</v>
+      </c>
+      <c r="J15" s="1">
+        <v>93.69</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N15" s="1">
         <v>2015</v>
       </c>
-      <c r="J15" s="1">
+      <c r="O15" s="1">
         <v>93</v>
       </c>
-      <c r="K15" s="1">
-        <v>93.69</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0.69</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P15" s="1">
+        <v>93.22</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0.219999999999999</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T15" s="1">
         <v>2015</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="U15" s="1">
         <v>93</v>
       </c>
-      <c r="R15" s="1">
-        <v>93.22</v>
-      </c>
-      <c r="S15" s="1">
-        <v>0.219999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V15" s="1">
+        <v>91.82</v>
+      </c>
+      <c r="W15" s="1">
+        <v>1.1800000000000099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1612,38 +1837,53 @@
       <c r="E16" s="1">
         <v>4.72</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>8</v>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2015</v>
       </c>
       <c r="I16" s="1">
+        <v>101</v>
+      </c>
+      <c r="J16" s="1">
+        <v>99.05</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N16" s="1">
         <v>2015</v>
       </c>
-      <c r="J16" s="1">
+      <c r="O16" s="1">
         <v>101</v>
       </c>
-      <c r="K16" s="1">
-        <v>99.05</v>
-      </c>
-      <c r="L16" s="1">
-        <v>1.95</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P16" s="1">
+        <v>97.32</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>3.6800000000000099</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T16" s="1">
         <v>2015</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="U16" s="1">
         <v>101</v>
       </c>
-      <c r="R16" s="1">
-        <v>97.32</v>
-      </c>
-      <c r="S16" s="1">
-        <v>3.6800000000000099</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V16" s="1">
+        <v>98.17</v>
+      </c>
+      <c r="W16" s="1">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1659,38 +1899,53 @@
       <c r="E17" s="1">
         <v>8.61</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>9</v>
+      <c r="G17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2015</v>
       </c>
       <c r="I17" s="1">
+        <v>100</v>
+      </c>
+      <c r="J17" s="1">
+        <v>92.74</v>
+      </c>
+      <c r="K17" s="1">
+        <v>7.26</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="1">
         <v>2015</v>
       </c>
-      <c r="J17" s="1">
+      <c r="O17" s="1">
         <v>100</v>
       </c>
-      <c r="K17" s="1">
-        <v>92.74</v>
-      </c>
-      <c r="L17" s="1">
-        <v>7.26</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P17" s="1">
+        <v>100.07</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>6.9999999999993207E-2</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T17" s="1">
         <v>2015</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="U17" s="1">
         <v>100</v>
       </c>
-      <c r="R17" s="1">
-        <v>100.07</v>
-      </c>
-      <c r="S17" s="1">
-        <v>6.9999999999993207E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V17" s="1">
+        <v>101.49</v>
+      </c>
+      <c r="W17" s="1">
+        <v>1.48999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1706,38 +1961,53 @@
       <c r="E18" s="1">
         <v>0.49</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>7</v>
+      <c r="G18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2016</v>
       </c>
       <c r="I18" s="1">
+        <v>95</v>
+      </c>
+      <c r="J18" s="1">
+        <v>96.87</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1.87</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="1">
         <v>2016</v>
       </c>
-      <c r="J18" s="1">
+      <c r="O18" s="1">
         <v>95</v>
       </c>
-      <c r="K18" s="1">
-        <v>96.87</v>
-      </c>
-      <c r="L18" s="1">
-        <v>1.87</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P18" s="1">
+        <v>94.23</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0.76999999999999602</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T18" s="1">
         <v>2016</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="U18" s="1">
         <v>95</v>
       </c>
-      <c r="R18" s="1">
-        <v>94.23</v>
-      </c>
-      <c r="S18" s="1">
-        <v>0.76999999999999602</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V18" s="1">
+        <v>92.31</v>
+      </c>
+      <c r="W18" s="1">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1753,38 +2023,53 @@
       <c r="E19" s="1">
         <v>0.66</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>8</v>
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2016</v>
       </c>
       <c r="I19" s="1">
+        <v>97</v>
+      </c>
+      <c r="J19" s="1">
+        <v>100.11</v>
+      </c>
+      <c r="K19" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N19" s="1">
         <v>2016</v>
       </c>
-      <c r="J19" s="1">
+      <c r="O19" s="1">
         <v>97</v>
       </c>
-      <c r="K19" s="1">
-        <v>100.11</v>
-      </c>
-      <c r="L19" s="1">
-        <v>3.11</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P19" s="1">
+        <v>98.7</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19" s="1">
         <v>2016</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="U19" s="1">
         <v>97</v>
       </c>
-      <c r="R19" s="1">
-        <v>98.7</v>
-      </c>
-      <c r="S19" s="1">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V19" s="1">
+        <v>97.53</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0.53000000000000103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1800,38 +2085,53 @@
       <c r="E20" s="1">
         <v>6.7</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>9</v>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2016</v>
       </c>
       <c r="I20" s="1">
+        <v>85</v>
+      </c>
+      <c r="J20" s="1">
+        <v>95.07</v>
+      </c>
+      <c r="K20" s="1">
+        <v>10.07</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="1">
         <v>2016</v>
       </c>
-      <c r="J20" s="1">
+      <c r="O20" s="1">
         <v>85</v>
       </c>
-      <c r="K20" s="1">
-        <v>95.07</v>
-      </c>
-      <c r="L20" s="1">
-        <v>10.07</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P20" s="1">
+        <v>89.67</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>4.67</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" s="1">
         <v>2016</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="U20" s="1">
         <v>85</v>
       </c>
-      <c r="R20" s="1">
-        <v>89.67</v>
-      </c>
-      <c r="S20" s="1">
-        <v>4.67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V20" s="1">
+        <v>90.44</v>
+      </c>
+      <c r="W20" s="1">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1847,38 +2147,53 @@
       <c r="E21" s="1">
         <v>3.61</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
+      <c r="G21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2017</v>
       </c>
       <c r="I21" s="1">
+        <v>99</v>
+      </c>
+      <c r="J21" s="1">
+        <v>95.14</v>
+      </c>
+      <c r="K21" s="1">
+        <v>3.86</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="1">
         <v>2017</v>
       </c>
-      <c r="J21" s="1">
+      <c r="O21" s="1">
         <v>99</v>
       </c>
-      <c r="K21" s="1">
-        <v>95.14</v>
-      </c>
-      <c r="L21" s="1">
-        <v>3.86</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P21" s="1">
+        <v>96.84</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>2.16</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T21" s="1">
         <v>2017</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="U21" s="1">
         <v>99</v>
       </c>
-      <c r="R21" s="1">
-        <v>96.84</v>
-      </c>
-      <c r="S21" s="1">
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V21" s="1">
+        <v>97.11</v>
+      </c>
+      <c r="W21" s="1">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1894,38 +2209,53 @@
       <c r="E22" s="1">
         <v>11.27</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>8</v>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2017</v>
       </c>
       <c r="I22" s="1">
+        <v>85</v>
+      </c>
+      <c r="J22" s="1">
+        <v>95.37</v>
+      </c>
+      <c r="K22" s="1">
+        <v>10.37</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N22" s="1">
         <v>2017</v>
       </c>
-      <c r="J22" s="1">
+      <c r="O22" s="1">
         <v>85</v>
       </c>
-      <c r="K22" s="1">
-        <v>95.37</v>
-      </c>
-      <c r="L22" s="1">
-        <v>10.37</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P22" s="1">
+        <v>87.89</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" s="1">
         <v>2017</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="U22" s="1">
         <v>85</v>
       </c>
-      <c r="R22" s="1">
-        <v>87.89</v>
-      </c>
-      <c r="S22" s="1">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V22" s="1">
+        <v>84.87</v>
+      </c>
+      <c r="W22" s="1">
+        <v>0.12999999999999501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1941,38 +2271,53 @@
       <c r="E23" s="1">
         <v>7.37</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>9</v>
+      <c r="G23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2017</v>
       </c>
       <c r="I23" s="1">
+        <v>84</v>
+      </c>
+      <c r="J23" s="1">
+        <v>95.22</v>
+      </c>
+      <c r="K23" s="1">
+        <v>11.22</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" s="1">
         <v>2017</v>
       </c>
-      <c r="J23" s="1">
+      <c r="O23" s="1">
         <v>84</v>
       </c>
-      <c r="K23" s="1">
-        <v>95.22</v>
-      </c>
-      <c r="L23" s="1">
-        <v>11.22</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P23" s="1">
+        <v>93.05</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T23" s="1">
         <v>2017</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="U23" s="1">
         <v>84</v>
       </c>
-      <c r="R23" s="1">
-        <v>93.05</v>
-      </c>
-      <c r="S23" s="1">
-        <v>9.0500000000000007</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V23" s="1">
+        <v>90.74</v>
+      </c>
+      <c r="W23" s="1">
+        <v>6.7399999999999904</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1988,38 +2333,53 @@
       <c r="E24" s="1">
         <v>6.41</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>7</v>
+      <c r="G24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2018</v>
       </c>
       <c r="I24" s="1">
+        <v>89</v>
+      </c>
+      <c r="J24" s="1">
+        <v>93.29</v>
+      </c>
+      <c r="K24" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="1">
         <v>2018</v>
       </c>
-      <c r="J24" s="1">
+      <c r="O24" s="1">
         <v>89</v>
       </c>
-      <c r="K24" s="1">
-        <v>93.29</v>
-      </c>
-      <c r="L24" s="1">
-        <v>4.29</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P24" s="1">
+        <v>93.23</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T24" s="1">
         <v>2018</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="U24" s="1">
         <v>89</v>
       </c>
-      <c r="R24" s="1">
-        <v>93.23</v>
-      </c>
-      <c r="S24" s="1">
-        <v>4.2300000000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V24" s="1">
+        <v>92.58</v>
+      </c>
+      <c r="W24" s="1">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -2035,38 +2395,53 @@
       <c r="E25" s="1">
         <v>2.1800000000000002</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>8</v>
+      <c r="G25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2018</v>
       </c>
       <c r="I25" s="1">
+        <v>98</v>
+      </c>
+      <c r="J25" s="1">
+        <v>95.42</v>
+      </c>
+      <c r="K25" s="1">
+        <v>2.58</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" s="1">
         <v>2018</v>
       </c>
-      <c r="J25" s="1">
+      <c r="O25" s="1">
         <v>98</v>
       </c>
-      <c r="K25" s="1">
-        <v>95.42</v>
-      </c>
-      <c r="L25" s="1">
-        <v>2.58</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P25" s="1">
+        <v>104.36</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>6.36</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T25" s="1">
         <v>2018</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="U25" s="1">
         <v>98</v>
       </c>
-      <c r="R25" s="1">
-        <v>104.36</v>
-      </c>
-      <c r="S25" s="1">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V25" s="1">
+        <v>104.99</v>
+      </c>
+      <c r="W25" s="1">
+        <v>6.9899999999999904</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -2082,38 +2457,53 @@
       <c r="E26" s="1">
         <v>3.99</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>9</v>
+      <c r="G26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2018</v>
       </c>
       <c r="I26" s="1">
+        <v>95</v>
+      </c>
+      <c r="J26" s="1">
+        <v>94.47</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="1">
         <v>2018</v>
       </c>
-      <c r="J26" s="1">
+      <c r="O26" s="1">
         <v>95</v>
       </c>
-      <c r="K26" s="1">
-        <v>94.47</v>
-      </c>
-      <c r="L26" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P26" s="1">
+        <v>94.55</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>0.45000000000000301</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T26" s="1">
         <v>2018</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="U26" s="1">
         <v>95</v>
       </c>
-      <c r="R26" s="1">
-        <v>94.55</v>
-      </c>
-      <c r="S26" s="1">
-        <v>0.45000000000000301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V26" s="1">
+        <v>90.9</v>
+      </c>
+      <c r="W26" s="1">
+        <v>4.0999999999999899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -2129,38 +2519,53 @@
       <c r="E27" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>7</v>
+      <c r="G27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2019</v>
       </c>
       <c r="I27" s="1">
+        <v>95</v>
+      </c>
+      <c r="J27" s="1">
+        <v>95.46</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="1">
         <v>2019</v>
       </c>
-      <c r="J27" s="1">
+      <c r="O27" s="1">
         <v>95</v>
       </c>
-      <c r="K27" s="1">
-        <v>95.46</v>
-      </c>
-      <c r="L27" s="1">
-        <v>0.46</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P27" s="1">
+        <v>94.19</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>0.81000000000000205</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T27" s="1">
         <v>2019</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="U27" s="1">
         <v>95</v>
       </c>
-      <c r="R27" s="1">
-        <v>94.19</v>
-      </c>
-      <c r="S27" s="1">
-        <v>0.81000000000000205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V27" s="1">
+        <v>91.39</v>
+      </c>
+      <c r="W27" s="1">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -2176,38 +2581,53 @@
       <c r="E28" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>8</v>
+      <c r="G28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2019</v>
       </c>
       <c r="I28" s="1">
+        <v>86</v>
+      </c>
+      <c r="J28" s="1">
+        <v>96.94</v>
+      </c>
+      <c r="K28" s="1">
+        <v>10.94</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N28" s="1">
         <v>2019</v>
       </c>
-      <c r="J28" s="1">
+      <c r="O28" s="1">
         <v>86</v>
       </c>
-      <c r="K28" s="1">
-        <v>96.94</v>
-      </c>
-      <c r="L28" s="1">
-        <v>10.94</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P28" s="1">
+        <v>88.29</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>2.2900000000000098</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T28" s="1">
         <v>2019</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="U28" s="1">
         <v>86</v>
       </c>
-      <c r="R28" s="1">
-        <v>88.29</v>
-      </c>
-      <c r="S28" s="1">
-        <v>2.2900000000000098</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V28" s="1">
+        <v>87.63</v>
+      </c>
+      <c r="W28" s="1">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -2223,38 +2643,53 @@
       <c r="E29" s="1">
         <v>0.12</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>9</v>
+      <c r="G29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2019</v>
       </c>
       <c r="I29" s="1">
+        <v>91</v>
+      </c>
+      <c r="J29" s="1">
+        <v>93.93</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2.93</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N29" s="1">
         <v>2019</v>
       </c>
-      <c r="J29" s="1">
+      <c r="O29" s="1">
         <v>91</v>
       </c>
-      <c r="K29" s="1">
-        <v>93.93</v>
-      </c>
-      <c r="L29" s="1">
-        <v>2.93</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P29" s="1">
+        <v>96.47</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>5.47</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T29" s="1">
         <v>2019</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="U29" s="1">
         <v>91</v>
       </c>
-      <c r="R29" s="1">
-        <v>96.47</v>
-      </c>
-      <c r="S29" s="1">
-        <v>5.47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V29" s="1">
+        <v>95.75</v>
+      </c>
+      <c r="W29" s="1">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -2270,38 +2705,53 @@
       <c r="E30" s="1">
         <v>3.05</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>7</v>
+      <c r="G30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2020</v>
       </c>
       <c r="I30" s="1">
+        <v>92</v>
+      </c>
+      <c r="J30" s="1">
+        <v>95.98</v>
+      </c>
+      <c r="K30" s="1">
+        <v>3.98</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="1">
         <v>2020</v>
       </c>
-      <c r="J30" s="1">
+      <c r="O30" s="1">
         <v>92</v>
       </c>
-      <c r="K30" s="1">
-        <v>95.98</v>
-      </c>
-      <c r="L30" s="1">
-        <v>3.98</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P30" s="1">
+        <v>93.9</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>1.9000000000000099</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T30" s="1">
         <v>2020</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="U30" s="1">
         <v>92</v>
       </c>
-      <c r="R30" s="1">
-        <v>93.9</v>
-      </c>
-      <c r="S30" s="1">
-        <v>1.9000000000000099</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V30" s="1">
+        <v>90.83</v>
+      </c>
+      <c r="W30" s="1">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -2317,38 +2767,53 @@
       <c r="E31" s="1">
         <v>18.39</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>8</v>
+      <c r="G31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2020</v>
       </c>
       <c r="I31" s="1">
+        <v>77</v>
+      </c>
+      <c r="J31" s="1">
+        <v>94.87</v>
+      </c>
+      <c r="K31" s="1">
+        <v>17.87</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N31" s="1">
         <v>2020</v>
       </c>
-      <c r="J31" s="1">
+      <c r="O31" s="1">
         <v>77</v>
       </c>
-      <c r="K31" s="1">
-        <v>94.87</v>
-      </c>
-      <c r="L31" s="1">
-        <v>17.87</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P31" s="1">
+        <v>91.77</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>14.77</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T31" s="1">
         <v>2020</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="U31" s="1">
         <v>77</v>
       </c>
-      <c r="R31" s="1">
-        <v>91.77</v>
-      </c>
-      <c r="S31" s="1">
-        <v>14.77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V31" s="1">
+        <v>89.89</v>
+      </c>
+      <c r="W31" s="1">
+        <v>12.89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -2364,38 +2829,53 @@
       <c r="E32" s="1">
         <v>11.06</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>9</v>
+      <c r="G32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2020</v>
       </c>
       <c r="I32" s="1">
+        <v>80</v>
+      </c>
+      <c r="J32" s="1">
+        <v>94.99</v>
+      </c>
+      <c r="K32" s="1">
+        <v>14.99</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="1">
         <v>2020</v>
       </c>
-      <c r="J32" s="1">
+      <c r="O32" s="1">
         <v>80</v>
       </c>
-      <c r="K32" s="1">
-        <v>94.99</v>
-      </c>
-      <c r="L32" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P32" s="1">
+        <v>85.24</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>5.2399999999999904</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T32" s="1">
         <v>2020</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="U32" s="1">
         <v>80</v>
       </c>
-      <c r="R32" s="1">
-        <v>85.24</v>
-      </c>
-      <c r="S32" s="1">
-        <v>5.2399999999999904</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V32" s="1">
+        <v>81.86</v>
+      </c>
+      <c r="W32" s="1">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -2411,38 +2891,53 @@
       <c r="E33" s="1">
         <v>9.8800000000000008</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>7</v>
+      <c r="G33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2021</v>
       </c>
       <c r="I33" s="1">
+        <v>85</v>
+      </c>
+      <c r="J33" s="1">
+        <v>96.1</v>
+      </c>
+      <c r="K33" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="1">
         <v>2021</v>
       </c>
-      <c r="J33" s="1">
+      <c r="O33" s="1">
         <v>85</v>
       </c>
-      <c r="K33" s="1">
-        <v>96.1</v>
-      </c>
-      <c r="L33" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="P33" s="1">
+        <v>92.75</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T33" s="1">
         <v>2021</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="U33" s="1">
         <v>85</v>
       </c>
-      <c r="R33" s="1">
-        <v>92.75</v>
-      </c>
-      <c r="S33" s="1">
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V33" s="1">
+        <v>90.75</v>
+      </c>
+      <c r="W33" s="1">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -2458,38 +2953,53 @@
       <c r="E34" s="1">
         <v>7.72</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>8</v>
+      <c r="G34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2021</v>
       </c>
       <c r="I34" s="1">
+        <v>87</v>
+      </c>
+      <c r="J34" s="1">
+        <v>99.02</v>
+      </c>
+      <c r="K34" s="1">
+        <v>12.02</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" s="1">
         <v>2021</v>
       </c>
-      <c r="J34" s="1">
+      <c r="O34" s="1">
         <v>87</v>
       </c>
-      <c r="K34" s="1">
-        <v>99.02</v>
-      </c>
-      <c r="L34" s="1">
-        <v>12.02</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="P34" s="1">
+        <v>97.46</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>10.46</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T34" s="1">
         <v>2021</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="U34" s="1">
         <v>87</v>
       </c>
-      <c r="R34" s="1">
-        <v>97.46</v>
-      </c>
-      <c r="S34" s="1">
-        <v>10.46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V34" s="1">
+        <v>96.28</v>
+      </c>
+      <c r="W34" s="1">
+        <v>9.2799999999999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -2505,54 +3015,74 @@
       <c r="E35" s="1">
         <v>3.56</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>9</v>
+      <c r="G35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2021</v>
       </c>
       <c r="I35" s="1">
+        <v>87</v>
+      </c>
+      <c r="J35" s="1">
+        <v>92.88</v>
+      </c>
+      <c r="K35" s="1">
+        <v>5.88</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" s="1">
         <v>2021</v>
       </c>
-      <c r="J35" s="1">
+      <c r="O35" s="1">
         <v>87</v>
       </c>
-      <c r="K35" s="1">
-        <v>92.88</v>
-      </c>
-      <c r="L35" s="1">
-        <v>5.88</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P35" s="1">
+        <v>90.44</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T35" s="1">
         <v>2021</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="U35" s="1">
         <v>87</v>
       </c>
-      <c r="R35" s="1">
-        <v>90.44</v>
-      </c>
-      <c r="S35" s="1">
-        <v>3.44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V35" s="1">
+        <v>89.36</v>
+      </c>
+      <c r="W35" s="1">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>201.46</v>
       </c>
-      <c r="L37">
+      <c r="K37">
         <v>196.26</v>
       </c>
-      <c r="S37">
-        <f>SUM(S3:S35)</f>
+      <c r="Q37">
+        <f>SUM(Q3:Q35)</f>
         <v>119.49000000000001</v>
       </c>
+      <c r="W37">
+        <f>SUM(W3:W35)</f>
+        <v>104.86999999999995</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="S1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>